<commit_message>
Updated documentation for v1.2.0
</commit_message>
<xml_diff>
--- a/Documents/UV-5R Radio Configuration Table.xlsx
+++ b/Documents/UV-5R Radio Configuration Table.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelnetherway/GitWorkspace/UV-5R/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_GitWorkspace\UV-5R\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F1AF25-D661-F447-8D23-F607A724DAE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{162F1E5A-3F72-4559-849B-AF43353035FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" activeTab="1" xr2:uid="{2F353EC1-3109-4D44-9297-7AF6286BFB6D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17620" activeTab="2" xr2:uid="{2F353EC1-3109-4D44-9297-7AF6286BFB6D}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9DABE3F3-0A48-411F-A84F-91D359320ED7}"/>
   </bookViews>
   <sheets>
     <sheet name="v1.0.0" sheetId="1" r:id="rId1"/>
     <sheet name="v1.1.0" sheetId="2" r:id="rId2"/>
+    <sheet name="v1.2.0" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="48">
   <si>
     <t>Frequency</t>
   </si>
@@ -127,6 +129,57 @@
   </si>
   <si>
     <t>Low</t>
+  </si>
+  <si>
+    <t>PMR 01</t>
+  </si>
+  <si>
+    <t>NFM</t>
+  </si>
+  <si>
+    <t>PMR 02</t>
+  </si>
+  <si>
+    <t>PMR 03</t>
+  </si>
+  <si>
+    <t>PMR 04</t>
+  </si>
+  <si>
+    <t>PMR 05</t>
+  </si>
+  <si>
+    <t>PMR 06</t>
+  </si>
+  <si>
+    <t>PMR 07</t>
+  </si>
+  <si>
+    <t>PMR 08</t>
+  </si>
+  <si>
+    <t>PMR 09</t>
+  </si>
+  <si>
+    <t>PMR 10</t>
+  </si>
+  <si>
+    <t>PMR 11</t>
+  </si>
+  <si>
+    <t>PMR 12</t>
+  </si>
+  <si>
+    <t>PMR 13</t>
+  </si>
+  <si>
+    <t>PMR 14</t>
+  </si>
+  <si>
+    <t>PMR 15</t>
+  </si>
+  <si>
+    <t>PMR 16</t>
   </si>
 </sst>
 </file>
@@ -171,7 +224,70 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="42">
+  <dxfs count="63">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -312,56 +428,84 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9342197A-6855-3B4C-A36B-604B959961DA}" name="Table1" displayName="Table1" ref="B2:T23" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9342197A-6855-3B4C-A36B-604B959961DA}" name="Table1" displayName="Table1" ref="B2:T23" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
   <autoFilter ref="B2:T23" xr:uid="{C17D325A-F6CF-6E45-9E03-FE14ECED045B}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{0F0DC48D-C7E9-2A46-9DC7-3682F15B042D}" name="Location" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{7603A102-6E5C-B04B-9B6F-F26375C8A809}" name="Name" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{D51AFB5A-8923-D343-A4F7-DDFA3918C662}" name="Frequency" dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{D1223C4B-F031-E24C-9688-0321238B20B5}" name="Duplex" dataDxfId="36"/>
-    <tableColumn id="5" xr3:uid="{2E00CBBA-E069-034F-9DC4-8BF666A00DF6}" name="Offset" dataDxfId="35"/>
-    <tableColumn id="6" xr3:uid="{A6FDE082-7974-BA41-BFB8-5A9A12C6D07E}" name="Tone" dataDxfId="34"/>
-    <tableColumn id="7" xr3:uid="{FFE6335B-DC58-F94B-AB2C-8E23EAB1DBAC}" name="rToneFreq" dataDxfId="33"/>
-    <tableColumn id="8" xr3:uid="{90515244-BB70-0A42-9A2F-C54C8FC54C1A}" name="cToneFreq" dataDxfId="32"/>
-    <tableColumn id="9" xr3:uid="{0F4818F0-2E06-E346-97C5-C49340C88242}" name="DtcsCode" dataDxfId="31"/>
-    <tableColumn id="10" xr3:uid="{44EDBCB0-85A9-9948-8B6D-B9E561A84C27}" name="DtcsPolarity" dataDxfId="30"/>
-    <tableColumn id="11" xr3:uid="{CA847C26-C577-DB42-83D4-EFD10E64EBEA}" name="Mode" dataDxfId="29"/>
-    <tableColumn id="12" xr3:uid="{5A376B5B-76D9-F64A-9ACF-EB6D64657AE3}" name="TStep" dataDxfId="28"/>
-    <tableColumn id="19" xr3:uid="{F0B0C53A-4E20-664F-9850-FF26529352BC}" name="Power" dataDxfId="27"/>
-    <tableColumn id="13" xr3:uid="{81B663FC-DA31-F04F-BAA9-4D3C64225DEE}" name="Skip" dataDxfId="26"/>
-    <tableColumn id="14" xr3:uid="{72F0A697-99B8-5745-88BE-BDE0C988CF0F}" name="Comment" dataDxfId="25"/>
-    <tableColumn id="15" xr3:uid="{DA27DEA7-3387-934B-83C4-0B303EF79DD1}" name="URCALL" dataDxfId="24"/>
-    <tableColumn id="16" xr3:uid="{A24B1DFA-03D0-534B-BA02-4BB0F5916144}" name="RPT1CALL" dataDxfId="23"/>
-    <tableColumn id="17" xr3:uid="{94278AE7-9F61-F443-8905-2766BA862444}" name="RPT2CALL" dataDxfId="22"/>
-    <tableColumn id="18" xr3:uid="{3CB3454E-0AFE-2145-8612-3D407DE21899}" name="DVCODE" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{0F0DC48D-C7E9-2A46-9DC7-3682F15B042D}" name="Location" dataDxfId="60"/>
+    <tableColumn id="2" xr3:uid="{7603A102-6E5C-B04B-9B6F-F26375C8A809}" name="Name" dataDxfId="59"/>
+    <tableColumn id="3" xr3:uid="{D51AFB5A-8923-D343-A4F7-DDFA3918C662}" name="Frequency" dataDxfId="58"/>
+    <tableColumn id="4" xr3:uid="{D1223C4B-F031-E24C-9688-0321238B20B5}" name="Duplex" dataDxfId="57"/>
+    <tableColumn id="5" xr3:uid="{2E00CBBA-E069-034F-9DC4-8BF666A00DF6}" name="Offset" dataDxfId="56"/>
+    <tableColumn id="6" xr3:uid="{A6FDE082-7974-BA41-BFB8-5A9A12C6D07E}" name="Tone" dataDxfId="55"/>
+    <tableColumn id="7" xr3:uid="{FFE6335B-DC58-F94B-AB2C-8E23EAB1DBAC}" name="rToneFreq" dataDxfId="54"/>
+    <tableColumn id="8" xr3:uid="{90515244-BB70-0A42-9A2F-C54C8FC54C1A}" name="cToneFreq" dataDxfId="53"/>
+    <tableColumn id="9" xr3:uid="{0F4818F0-2E06-E346-97C5-C49340C88242}" name="DtcsCode" dataDxfId="52"/>
+    <tableColumn id="10" xr3:uid="{44EDBCB0-85A9-9948-8B6D-B9E561A84C27}" name="DtcsPolarity" dataDxfId="51"/>
+    <tableColumn id="11" xr3:uid="{CA847C26-C577-DB42-83D4-EFD10E64EBEA}" name="Mode" dataDxfId="50"/>
+    <tableColumn id="12" xr3:uid="{5A376B5B-76D9-F64A-9ACF-EB6D64657AE3}" name="TStep" dataDxfId="49"/>
+    <tableColumn id="19" xr3:uid="{F0B0C53A-4E20-664F-9850-FF26529352BC}" name="Power" dataDxfId="48"/>
+    <tableColumn id="13" xr3:uid="{81B663FC-DA31-F04F-BAA9-4D3C64225DEE}" name="Skip" dataDxfId="47"/>
+    <tableColumn id="14" xr3:uid="{72F0A697-99B8-5745-88BE-BDE0C988CF0F}" name="Comment" dataDxfId="46"/>
+    <tableColumn id="15" xr3:uid="{DA27DEA7-3387-934B-83C4-0B303EF79DD1}" name="URCALL" dataDxfId="45"/>
+    <tableColumn id="16" xr3:uid="{A24B1DFA-03D0-534B-BA02-4BB0F5916144}" name="RPT1CALL" dataDxfId="44"/>
+    <tableColumn id="17" xr3:uid="{94278AE7-9F61-F443-8905-2766BA862444}" name="RPT2CALL" dataDxfId="43"/>
+    <tableColumn id="18" xr3:uid="{3CB3454E-0AFE-2145-8612-3D407DE21899}" name="DVCODE" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A35C8064-2C76-1741-8D6D-007C7AE794EF}" name="Table2" displayName="Table2" ref="B2:T10" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A35C8064-2C76-1741-8D6D-007C7AE794EF}" name="Table2" displayName="Table2" ref="B2:T10" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <autoFilter ref="B2:T10" xr:uid="{03D48D7C-A000-1E46-B6BB-418101329904}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{DC76DF2C-1854-B149-BA13-48EF14F94411}" name="Location" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{B6654602-8492-7241-8E02-D27F8AABD411}" name="Name" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{6CD54839-5F38-4645-A304-FC949F49AD0B}" name="Frequency" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{0290EE6A-9A94-E645-AB7E-A10F786E33B7}" name="Duplex" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{287F5C26-4BAA-3949-8D55-A149745CDC30}" name="Offset" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{1531338C-3A3D-6443-AF01-A54F320D1C2A}" name="Tone" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{3102D285-4DD4-D74C-8568-AC0A061B5C80}" name="rToneFreq" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{ED1E9804-BF0F-604D-A125-454365AAF4E1}" name="cToneFreq" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{11D5D276-5AFF-5F4D-AA7E-FA65B57749BD}" name="DtcsCode" dataDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{B1052BDB-D80B-C844-9EFD-F5C50CB97F1A}" name="DtcsPolarity" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{9BCA39F8-E4FD-B143-A5FF-E33B00752993}" name="Mode" dataDxfId="10"/>
-    <tableColumn id="12" xr3:uid="{E999DEED-6531-D84D-9658-CB64495344D5}" name="TStep" dataDxfId="9"/>
-    <tableColumn id="19" xr3:uid="{4FBBBDF6-DE8E-4741-8886-5542B5AD5EC6}" name="Power" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{80BBB55D-9F71-6C40-A2BF-D64CC876D749}" name="Skip" dataDxfId="7"/>
-    <tableColumn id="14" xr3:uid="{118D24B4-9D6D-4E40-8232-61F48D3F2F86}" name="Comment" dataDxfId="6"/>
-    <tableColumn id="15" xr3:uid="{518AE64F-A3AC-5E44-9CDA-64B769ABACC5}" name="URCALL" dataDxfId="5"/>
-    <tableColumn id="16" xr3:uid="{8E2B87FA-C515-8748-8790-1D7551E2BD11}" name="RPT1CALL" dataDxfId="4"/>
-    <tableColumn id="17" xr3:uid="{EF49AF01-0F26-9141-8171-88D1F314F819}" name="RPT2CALL" dataDxfId="3"/>
-    <tableColumn id="18" xr3:uid="{DDECAFA5-E3B7-454D-B253-022558573AD4}" name="DVCODE" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{DC76DF2C-1854-B149-BA13-48EF14F94411}" name="Location" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{B6654602-8492-7241-8E02-D27F8AABD411}" name="Name" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{6CD54839-5F38-4645-A304-FC949F49AD0B}" name="Frequency" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{0290EE6A-9A94-E645-AB7E-A10F786E33B7}" name="Duplex" dataDxfId="36"/>
+    <tableColumn id="5" xr3:uid="{287F5C26-4BAA-3949-8D55-A149745CDC30}" name="Offset" dataDxfId="35"/>
+    <tableColumn id="6" xr3:uid="{1531338C-3A3D-6443-AF01-A54F320D1C2A}" name="Tone" dataDxfId="34"/>
+    <tableColumn id="7" xr3:uid="{3102D285-4DD4-D74C-8568-AC0A061B5C80}" name="rToneFreq" dataDxfId="33"/>
+    <tableColumn id="8" xr3:uid="{ED1E9804-BF0F-604D-A125-454365AAF4E1}" name="cToneFreq" dataDxfId="32"/>
+    <tableColumn id="9" xr3:uid="{11D5D276-5AFF-5F4D-AA7E-FA65B57749BD}" name="DtcsCode" dataDxfId="31"/>
+    <tableColumn id="10" xr3:uid="{B1052BDB-D80B-C844-9EFD-F5C50CB97F1A}" name="DtcsPolarity" dataDxfId="30"/>
+    <tableColumn id="11" xr3:uid="{9BCA39F8-E4FD-B143-A5FF-E33B00752993}" name="Mode" dataDxfId="29"/>
+    <tableColumn id="12" xr3:uid="{E999DEED-6531-D84D-9658-CB64495344D5}" name="TStep" dataDxfId="28"/>
+    <tableColumn id="19" xr3:uid="{4FBBBDF6-DE8E-4741-8886-5542B5AD5EC6}" name="Power" dataDxfId="27"/>
+    <tableColumn id="13" xr3:uid="{80BBB55D-9F71-6C40-A2BF-D64CC876D749}" name="Skip" dataDxfId="26"/>
+    <tableColumn id="14" xr3:uid="{118D24B4-9D6D-4E40-8232-61F48D3F2F86}" name="Comment" dataDxfId="25"/>
+    <tableColumn id="15" xr3:uid="{518AE64F-A3AC-5E44-9CDA-64B769ABACC5}" name="URCALL" dataDxfId="24"/>
+    <tableColumn id="16" xr3:uid="{8E2B87FA-C515-8748-8790-1D7551E2BD11}" name="RPT1CALL" dataDxfId="23"/>
+    <tableColumn id="17" xr3:uid="{EF49AF01-0F26-9141-8171-88D1F314F819}" name="RPT2CALL" dataDxfId="22"/>
+    <tableColumn id="18" xr3:uid="{DDECAFA5-E3B7-454D-B253-022558573AD4}" name="DVCODE" dataDxfId="21"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A41059B2-BC0A-401C-A02F-D8C7B9499AF9}" name="Table3" displayName="Table3" ref="B2:T18" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="B2:T18" xr:uid="{943E5013-54F9-4E82-AD5A-E0DC19EA09B5}"/>
+  <tableColumns count="19">
+    <tableColumn id="1" xr3:uid="{E0E0F7E8-9E54-4666-B0A6-DBB94ABFCEEA}" name="Location" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{A1357C04-1255-4527-8A9F-1D81840018CA}" name="Name" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{6566C813-3671-4FDC-98B6-1BF2A9811CAB}" name="Frequency" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{73EB66A6-DF8D-4B0C-8247-A672E2E303F9}" name="Duplex" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{7DF53FE7-E0B6-4A3E-8478-E55353F78312}" name="Offset" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{C33606E1-CEDE-4CF6-A893-150D930C96DF}" name="Tone" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{42A6218E-91AF-4502-8CF9-3AFB1ABDF6C7}" name="rToneFreq" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{90A5B14B-9C1C-406D-9CAE-2AE83CBF2B60}" name="cToneFreq" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{BCE7B94E-56BB-4A6B-B7E0-73CE30B5F286}" name="DtcsCode" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{3E998DCC-B518-42AF-981C-22D426C2F84D}" name="DtcsPolarity" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{E3C50708-5E72-45A6-998C-4B2ADE74328E}" name="Mode" dataDxfId="10"/>
+    <tableColumn id="12" xr3:uid="{112735BA-A15E-40E5-BCB2-5E6BEC3DB664}" name="TStep" dataDxfId="9"/>
+    <tableColumn id="19" xr3:uid="{659E5826-CF86-4DFE-B55B-24DD9D1F435F}" name="Power" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{51D687AB-FEF2-419F-B89C-671E22DEEDAB}" name="Skip" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{EAF2E168-8334-40F3-8D70-94903EE52B2D}" name="Comment" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{0F61FBA3-6306-4092-9AED-6F7F336903C0}" name="URCALL" dataDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{503D8B5A-93B3-43AD-AB41-D02AD32DFC03}" name="RPT1CALL" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{0378E862-14C8-453D-85E7-BD37CBD79583}" name="RPT2CALL" dataDxfId="3"/>
+    <tableColumn id="18" xr3:uid="{55982A4D-D7AA-4972-B078-BC36FDE74D79}" name="DVCODE" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -669,8 +813,9 @@
     <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
@@ -691,7 +836,7 @@
     <col min="20" max="20" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
@@ -750,7 +895,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -791,7 +936,7 @@
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
     </row>
-    <row r="4" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B4" s="1">
         <v>2</v>
       </c>
@@ -832,7 +977,7 @@
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
     </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -873,7 +1018,7 @@
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
     </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B6" s="1">
         <v>4</v>
       </c>
@@ -914,7 +1059,7 @@
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
     </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B7" s="1">
         <v>5</v>
       </c>
@@ -955,7 +1100,7 @@
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
     </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B8" s="1">
         <v>6</v>
       </c>
@@ -996,7 +1141,7 @@
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
     </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B9" s="1">
         <v>7</v>
       </c>
@@ -1037,7 +1182,7 @@
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
     </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B10" s="1">
         <v>8</v>
       </c>
@@ -1078,7 +1223,7 @@
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
     </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B11" s="1">
         <v>9</v>
       </c>
@@ -1119,7 +1264,7 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
     </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B12" s="1">
         <v>10</v>
       </c>
@@ -1160,7 +1305,7 @@
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
     </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B13" s="1">
         <v>11</v>
       </c>
@@ -1201,7 +1346,7 @@
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
     </row>
-    <row r="14" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B14" s="1">
         <v>12</v>
       </c>
@@ -1242,7 +1387,7 @@
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
     </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B15" s="1">
         <v>13</v>
       </c>
@@ -1283,7 +1428,7 @@
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
     </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B16" s="1">
         <v>14</v>
       </c>
@@ -1324,7 +1469,7 @@
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
     </row>
-    <row r="17" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B17" s="1">
         <v>15</v>
       </c>
@@ -1365,7 +1510,7 @@
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
     </row>
-    <row r="18" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B18" s="1">
         <v>16</v>
       </c>
@@ -1406,7 +1551,7 @@
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
     </row>
-    <row r="19" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B19" s="1">
         <v>17</v>
       </c>
@@ -1447,7 +1592,7 @@
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
     </row>
-    <row r="20" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B20" s="1">
         <v>18</v>
       </c>
@@ -1488,7 +1633,7 @@
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
     </row>
-    <row r="21" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B21" s="1">
         <v>19</v>
       </c>
@@ -1529,7 +1674,7 @@
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
     </row>
-    <row r="22" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B22" s="1">
         <v>20</v>
       </c>
@@ -1570,7 +1715,7 @@
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
     </row>
-    <row r="23" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B23" s="1">
         <v>21</v>
       </c>
@@ -1623,11 +1768,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C10B9412-18EF-8C49-AB6A-5D98372D5E9F}">
   <dimension ref="B2:T10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
@@ -1648,7 +1794,7 @@
     <col min="20" max="20" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1707,7 +1853,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -1750,7 +1896,7 @@
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
     </row>
-    <row r="4" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B4" s="1">
         <v>2</v>
       </c>
@@ -1793,7 +1939,7 @@
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
     </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -1836,7 +1982,7 @@
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
     </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B6" s="1">
         <v>4</v>
       </c>
@@ -1879,7 +2025,7 @@
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
     </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B7" s="1">
         <v>5</v>
       </c>
@@ -1922,7 +2068,7 @@
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
     </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B8" s="1">
         <v>6</v>
       </c>
@@ -1965,7 +2111,7 @@
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
     </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B9" s="1">
         <v>7</v>
       </c>
@@ -2008,7 +2154,7 @@
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
     </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B10" s="1">
         <v>8</v>
       </c>
@@ -2050,6 +2196,792 @@
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45814495-0B45-41E6-AEE9-DE95E801D23D}">
+  <dimension ref="B2:T18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.9140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.58203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.08203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.08203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.58203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.58203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.4140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.4140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="1">
+        <v>446.00625000000002</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I3" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J3" s="1">
+        <v>23</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" s="1">
+        <v>5</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="1">
+        <v>446.01875000000001</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I4" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J4" s="1">
+        <v>23</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" s="1">
+        <v>5</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="1">
+        <v>446.03125</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I5" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J5" s="1">
+        <v>23</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M5" s="1">
+        <v>5</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="1">
+        <v>446.04374999999999</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I6" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J6" s="1">
+        <v>23</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M6" s="1">
+        <v>5</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B7" s="1">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="1">
+        <v>446.05624999999998</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I7" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J7" s="1">
+        <v>23</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M7" s="1">
+        <v>5</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B8" s="1">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="1">
+        <v>446.06875000000002</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I8" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J8" s="1">
+        <v>23</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M8" s="1">
+        <v>5</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B9" s="1">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="1">
+        <v>446.08125000000001</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I9" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J9" s="1">
+        <v>23</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M9" s="1">
+        <v>5</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B10" s="1">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="1">
+        <v>446.09375</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I10" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J10" s="1">
+        <v>23</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M10" s="1">
+        <v>5</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B11" s="1">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="1">
+        <v>446.10624999999999</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I11" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J11" s="1">
+        <v>23</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M11" s="1">
+        <v>5</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B12" s="1">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="1">
+        <v>446.11874999999998</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I12" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J12" s="1">
+        <v>23</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M12" s="1">
+        <v>5</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B13" s="1">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="1">
+        <v>446.13125000000002</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I13" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J13" s="1">
+        <v>23</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M13" s="1">
+        <v>5</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B14" s="1">
+        <v>12</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="1">
+        <v>446.14375000000001</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I14" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J14" s="1">
+        <v>23</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M14" s="1">
+        <v>5</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B15" s="1">
+        <v>13</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="1">
+        <v>446.15625</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I15" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J15" s="1">
+        <v>23</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M15" s="1">
+        <v>5</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B16" s="1">
+        <v>14</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="1">
+        <v>446.16874999999999</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I16" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J16" s="1">
+        <v>23</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M16" s="1">
+        <v>5</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B17" s="1">
+        <v>15</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="1">
+        <v>446.18124999999998</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I17" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J17" s="1">
+        <v>23</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M17" s="1">
+        <v>5</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B18" s="1">
+        <v>16</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="1">
+        <v>446.19375000000002</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="I18" s="1">
+        <v>88.5</v>
+      </c>
+      <c r="J18" s="1">
+        <v>23</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M18" s="1">
+        <v>5</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>